<commit_message>
Incluidos los archivos gerber
</commit_message>
<xml_diff>
--- a/BOM_Acelerómetro_ADXL345_AETEL.xlsx
+++ b/BOM_Acelerómetro_ADXL345_AETEL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>ITEM</t>
   </si>
@@ -75,27 +75,12 @@
     <t>BENEFIT</t>
   </si>
   <si>
-    <t>Converter € to $</t>
-  </si>
-  <si>
-    <t>Converter $ to €</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>OUT</t>
-  </si>
-  <si>
     <t>BOM AETEL ADXL345</t>
   </si>
   <si>
     <t>Placa AETEL-Sparkfun 2C Serigrafia- Máscara soldadura 20x15mm</t>
   </si>
   <si>
-    <t>STOCK Manuel</t>
-  </si>
-  <si>
     <t>http://es.aliexpress.com/store/product/5Pcs-ADXL345-ADXL345BCCZ-Inertial-sensor-3-axis-accelerometer-digital- accelerometer/511081_1695933338.html?spm=2114.04020208.3.1.St9qvK&amp;ws_ab_test=201556_7,201527_2_71_72_73_74_75,201560_9</t>
   </si>
   <si>
@@ -130,6 +115,9 @@
   </si>
   <si>
     <t>http://es.aliexpress.com/store/product/100g-Sn42Bi58-SD-528T-low-temperature-SMT-LED-leadfree-SMT-solder-paste/1303584_32233318638.html?spm=2114.04020208.3.11.oDRJdq&amp;ws_ab_test=201556_7,201527_2_71_72_73_74_75,201560_9</t>
+  </si>
+  <si>
+    <t>Manuel</t>
   </si>
 </sst>
 </file>
@@ -195,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,14 +232,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="19">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -371,132 +353,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -537,15 +399,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -848,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection sqref="A1:L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +724,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -925,7 +778,7 @@
     </row>
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -934,7 +787,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="8">
-        <f>ROUNDUP(((B3*$B$16)/C3),0)</f>
+        <f>ROUNDUP(((B3*$B$15)/C3),0)</f>
         <v>1</v>
       </c>
       <c r="E3" s="9">
@@ -960,16 +813,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="12">
-        <f>D3*C3 - B3*$B$16</f>
+        <f>D3*C3 - B3*$B$15</f>
         <v>20</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
@@ -978,11 +831,11 @@
         <v>10</v>
       </c>
       <c r="D4" s="8">
-        <f>ROUNDUP(((B4*$B$16)/C4),0)</f>
+        <f>ROUNDUP(((B4*$B$15)/C4),0)</f>
         <v>2</v>
       </c>
       <c r="E4" s="9">
-        <f>(F4/$B$17)</f>
+        <f>(F4/$B$16)</f>
         <v>5.3963963963963959</v>
       </c>
       <c r="F4" s="10">
@@ -1005,16 +858,16 @@
         <v>10.792792792792792</v>
       </c>
       <c r="K4" s="12">
-        <f>D4*C4 - B4*$B$16</f>
+        <f>D4*C4 - B4*$B$15</f>
         <v>0</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
@@ -1023,7 +876,7 @@
         <v>50</v>
       </c>
       <c r="D5" s="8">
-        <f>ROUNDUP(((B5*$B$16)/C5),0)</f>
+        <f>ROUNDUP(((B5*$B$15)/C5),0)</f>
         <v>1</v>
       </c>
       <c r="E5" s="9">
@@ -1049,16 +902,16 @@
         <v>2.08</v>
       </c>
       <c r="K5" s="12">
-        <f>D5*C5 - B5*$B$16</f>
+        <f>D5*C5 - B5*$B$15</f>
         <v>30</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
@@ -1067,7 +920,7 @@
         <v>100</v>
       </c>
       <c r="D6" s="8">
-        <f>ROUNDUP(((B6*$B$16)/C6),0)</f>
+        <f>ROUNDUP(((B6*$B$15)/C6),0)</f>
         <v>1</v>
       </c>
       <c r="E6" s="9">
@@ -1093,16 +946,16 @@
         <v>0.64</v>
       </c>
       <c r="K6" s="12">
-        <f>D6*C6 - B6*$B$16</f>
+        <f>D6*C6 - B6*$B$15</f>
         <v>60</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
@@ -1139,12 +992,12 @@
         <v>0</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
@@ -1181,12 +1034,12 @@
         <v>0</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
@@ -1223,126 +1076,127 @@
         <v>0</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="7"/>
+      <c r="A10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18">
+        <f>SUM(I3:I9)</f>
+        <v>20.534039639639641</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18">
-        <f>SUM(I3:I10)</f>
-        <v>20.534039639639641</v>
-      </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20"/>
+      <c r="A11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24">
+        <f>SUM(J3:J9)</f>
+        <v>33.452792792792792</v>
+      </c>
+      <c r="K11" s="25"/>
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23">
-        <f>J12/B16</f>
-        <v>1.6726396396396397</v>
-      </c>
-      <c r="J12" s="24">
-        <f>SUM(J3:J10)</f>
-        <v>33.452792792792792</v>
-      </c>
-      <c r="K12" s="25"/>
+      <c r="A12" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28">
+        <f>(B14*B15)</f>
+        <v>40</v>
+      </c>
+      <c r="K12" s="29"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28">
-        <f>(B15*B16)</f>
-        <v>40</v>
+      <c r="A13" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="32">
+        <f>J12-J11</f>
+        <v>6.5472072072072081</v>
       </c>
       <c r="K13" s="29"/>
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32">
-        <f>J13-J12</f>
-        <v>6.5472072072072081</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B14" s="33">
+        <v>2</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="35"/>
       <c r="K14" s="29"/>
       <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="33">
-        <v>2</v>
-      </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="29"/>
+      <c r="A15" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="37">
+        <v>20</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="37">
-        <v>20</v>
+    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="39">
+        <v>1.1100000000000001</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1355,101 +1209,25 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="39">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="44">
-        <v>0.06</v>
-      </c>
-      <c r="C19" s="45">
-        <f>B19*B17</f>
-        <v>6.6600000000000006E-2</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="48">
-        <f>B20/B17</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>